<commit_message>
changes in database, folder structure:added data folder for database design, sql files , added new CA exam feature
</commit_message>
<xml_diff>
--- a/yschool/src/main/webapp/spreadsheet-templates/start_ySchool.xlsx
+++ b/yschool/src/main/webapp/spreadsheet-templates/start_ySchool.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayrksih\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\yschoolnew\yschool\src\main\webapp\spreadsheet-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6285" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6285" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>Addmission No.</t>
   </si>
@@ -160,13 +160,49 @@
     <t>Science</t>
   </si>
   <si>
-    <t>tamil</t>
-  </si>
-  <si>
     <t>Thillaiyampathi</t>
   </si>
   <si>
     <t>Thilayampathi Saravanapperumal</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Tamil</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Gamage</t>
+  </si>
+  <si>
+    <t>Malaka</t>
+  </si>
+  <si>
+    <t>Dr chandana Gamage</t>
+  </si>
+  <si>
+    <t>Dr Malaka walapola</t>
   </si>
 </sst>
 </file>
@@ -524,6 +560,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -936,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -963,10 +1095,32 @@
         <v>43354</v>
       </c>
       <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
-        <v>32</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>12345</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>34567</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -977,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1014,10 +1168,42 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1034,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1061,7 +1247,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>2013</v>
@@ -1072,9 +1258,119 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="C6">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13">
         <v>2013</v>
       </c>
     </row>

</xml_diff>